<commit_message>
Input grid centorids for agricultural samples
</commit_message>
<xml_diff>
--- a/analysis/metadata/P08_8/P08_8_minimal_metadata.xlsx
+++ b/analysis/metadata/P08_8/P08_8_minimal_metadata.xlsx
@@ -473,17 +473,27 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
           <t>2022-09-21</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -521,17 +531,27 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>2022-09-21</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -569,17 +589,27 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>2022-09-18</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -617,17 +647,27 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
           <t>2022-09-17</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -665,17 +705,27 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>2022-09-17</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -713,17 +763,27 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>2022-09-18</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -761,17 +821,27 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
           <t>2022-09-18</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -809,17 +879,27 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
           <t>2022-10-02</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -857,17 +937,27 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>2022-09-18</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>
@@ -905,17 +995,27 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>soil</t>
+          <t>Soil</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>natural</t>
+          <t>Natural</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
           <t>2022-09-28</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
         </is>
       </c>
     </row>

</xml_diff>